<commit_message>
Client has the ability to choose between 3 Basic plans and the plans populate workout events on the calendar on there index page
</commit_message>
<xml_diff>
--- a/Planning Tools/SeededWorkouts.xlsx
+++ b/Planning Tools/SeededWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamm\OneDrive\Desktop\Matsusanity\Planning Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25AB5653-A922-44DD-A52E-D3EE46A54593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF392A4-D522-4A1A-8EE5-461A7D7E42A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E778A07-9D40-4287-921F-53580F58C7EF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Pull-ups</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>Client!123</t>
+  </si>
+  <si>
+    <t>Body-Weight Description</t>
+  </si>
+  <si>
+    <t>Body-Weight Workout</t>
+  </si>
+  <si>
+    <t>Upper Body Description</t>
+  </si>
+  <si>
+    <t>Upper Body</t>
+  </si>
+  <si>
+    <t>Lower Body Description</t>
+  </si>
+  <si>
+    <t>Lower Body</t>
   </si>
 </sst>
 </file>
@@ -141,9 +159,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,201 +483,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFAC23-610C-4B73-8EB7-4C99AE4F82F4}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E13:E14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>10</v>
-      </c>
       <c r="C1">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1">
-        <v>10</v>
-      </c>
       <c r="G1">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
       </c>
       <c r="K1">
-        <v>3</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>3</v>
       </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="N1">
-        <v>10</v>
-      </c>
       <c r="O1">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="P1">
+        <v>3</v>
       </c>
       <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
         <v>5</v>
       </c>
-      <c r="R1">
-        <v>10</v>
-      </c>
       <c r="S1">
-        <v>3</v>
-      </c>
-      <c r="T1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
       <c r="C2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>150</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
       <c r="G2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
       <c r="K2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
         <v>80</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>9</v>
       </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
       <c r="O2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
         <v>130</v>
       </c>
-      <c r="Q2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2">
+      <c r="R2" t="s">
         <v>10</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="T2">
+        <v>3</v>
+      </c>
+      <c r="U2">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
       <c r="C3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>180</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
       <c r="G3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
         <v>160</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
       <c r="K3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
         <v>85</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>14</v>
       </c>
-      <c r="N3">
-        <v>10</v>
-      </c>
       <c r="O3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
         <v>80</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>15</v>
       </c>
-      <c r="R3">
-        <v>10</v>
-      </c>
       <c r="S3">
-        <v>3</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -661,7 +694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -669,12 +702,75 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>43914</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43914.041666666664</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>43915</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43915.041666666664</v>
+      </c>
+      <c r="E14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>43916</v>
+      </c>
+      <c r="D15" s="3">
+        <v>43916.041666666664</v>
+      </c>
+      <c r="E15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clients can now add a chosen personal trainer to their profile
</commit_message>
<xml_diff>
--- a/Planning Tools/SeededWorkouts.xlsx
+++ b/Planning Tools/SeededWorkouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamm\OneDrive\Desktop\Matsusanity\Planning Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF392A4-D522-4A1A-8EE5-461A7D7E42A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67D9EEC-E2F7-4BA6-A240-1A345AE0492C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E778A07-9D40-4287-921F-53580F58C7EF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Pull-ups</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Lower Body</t>
+  </si>
+  <si>
+    <t>Stripe</t>
+  </si>
+  <si>
+    <t>matsusanity@gmail.com</t>
+  </si>
+  <si>
+    <t>Matsu123Sanity!</t>
   </si>
 </sst>
 </file>
@@ -483,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFAC23-610C-4B73-8EB7-4C99AE4F82F4}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,11 +782,27 @@
         <v>27</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{C83D1E49-FCE0-4037-9A3F-F89C7E48F001}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{7B0E6C65-FEE4-43BF-9DBA-0AA642CAAF65}"/>
     <hyperlink ref="A9" r:id="rId3" xr:uid="{477FBDCD-59AA-4809-9CC1-8DC76F8876E0}"/>
+    <hyperlink ref="A18" r:id="rId4" xr:uid="{1AC18EB9-CDAA-458B-AB0D-C7E37906E24A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>